<commit_message>
absolute mess. added plot_everything and mods
</commit_message>
<xml_diff>
--- a/reports/TS_Cyto_significant_times.xlsx
+++ b/reports/TS_Cyto_significant_times.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IL18_ATP" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IL18_MSU" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IL18_Nigericin" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IL1b_ATP" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IL1b_MSU" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IL1b_Nigericin" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="IL18_ATP" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="IL18_MSU" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="IL18_Nigericin" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="IL1b_ATP" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="IL1b_MSU" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="IL1b_Nigericin" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -490,14 +490,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>9.483:12.439</t>
+          <t>9.516:12.444</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.01</v>
+        <v>0.017</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01043478260869565</v>
+        <v>0.01773913043478261</v>
       </c>
       <c r="H2" t="n">
         <v>0.9</v>
@@ -518,14 +518,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>9.257:11.661</t>
+          <t>9.279:11.665</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.022</v>
+        <v>0.02</v>
       </c>
       <c r="G3" t="n">
-        <v>0.022</v>
+        <v>0.02</v>
       </c>
       <c r="H3" t="n">
         <v>0.9</v>
@@ -546,14 +546,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>9.885:13.285</t>
+          <t>9.85:13.267</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="G4" t="n">
-        <v>0.004363636363636364</v>
+        <v>0.0032</v>
       </c>
       <c r="H4" t="n">
         <v>0.9</v>
@@ -574,14 +574,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10.612:16.32</t>
+          <t>10.565:16.29</t>
         </is>
       </c>
       <c r="F5" t="n">
         <v>0.001</v>
       </c>
       <c r="G5" t="n">
-        <v>0.001714285714285714</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H5" t="n">
         <v>0.9</v>
@@ -602,14 +602,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>11.283:19.108</t>
+          <t>11.233:19.074</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="G6" t="n">
-        <v>0.002666666666666667</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H6" t="n">
         <v>0.9</v>
@@ -630,14 +630,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>11.909:22.154</t>
+          <t>12.098:22.077</t>
         </is>
       </c>
       <c r="F7" t="n">
         <v>0.001</v>
       </c>
       <c r="G7" t="n">
-        <v>0.001714285714285714</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H7" t="n">
         <v>0.9</v>
@@ -658,14 +658,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>12.678:24.398</t>
+          <t>12.637:24.461</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="G8" t="n">
-        <v>0.001714285714285714</v>
+        <v>0.004235294117647058</v>
       </c>
       <c r="H8" t="n">
         <v>0.9</v>
@@ -686,14 +686,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>13.37:27.667</t>
+          <t>13.343:27.638</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0036</v>
+        <v>0.004363636363636364</v>
       </c>
       <c r="H9" t="n">
         <v>0.9</v>
@@ -714,14 +714,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>13.898:29.265</t>
+          <t>14.029:29.271</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="G10" t="n">
-        <v>0.004363636363636364</v>
+        <v>0.004235294117647058</v>
       </c>
       <c r="H10" t="n">
         <v>0.9</v>
@@ -742,14 +742,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>14.171:32.128</t>
+          <t>14.491:32.095</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H11" t="n">
         <v>0.9</v>
@@ -770,14 +770,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>15.179:34.961</t>
+          <t>15.34:34.907</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0.001</v>
+        <v>0.004</v>
       </c>
       <c r="G12" t="n">
-        <v>0.001714285714285714</v>
+        <v>0.004363636363636364</v>
       </c>
       <c r="H12" t="n">
         <v>0.9</v>
@@ -798,14 +798,14 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>16.019:37.633</t>
+          <t>15.649:37.632</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G13" t="n">
-        <v>0.001714285714285714</v>
+        <v>0.0032</v>
       </c>
       <c r="H13" t="n">
         <v>0.9</v>
@@ -826,14 +826,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>16.444:41.62</t>
+          <t>16.656:41.709</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>0.0032</v>
       </c>
       <c r="H14" t="n">
         <v>0.9</v>
@@ -854,14 +854,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>17.281:43.464</t>
+          <t>17.223:43.521</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H15" t="n">
         <v>0.9</v>
@@ -882,14 +882,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>17.946:47.069</t>
+          <t>17.88:47.015</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.002</v>
+        <v>0.004</v>
       </c>
       <c r="G16" t="n">
-        <v>0.002666666666666667</v>
+        <v>0.004363636363636364</v>
       </c>
       <c r="H16" t="n">
         <v>0.9</v>
@@ -910,14 +910,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>18.729:52.109</t>
+          <t>18.751:51.775</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0.003</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0036</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
         <v>0.9</v>
@@ -938,14 +938,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>20.329:60.804</t>
+          <t>20.652:60.876</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.001714285714285714</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
         <v>0.9</v>
@@ -966,14 +966,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>22.67:71.049</t>
+          <t>22.695:70.817</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0.002666666666666667</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
         <v>0.9</v>
@@ -994,14 +994,14 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>22.497:68.924</t>
+          <t>22.296:69.11</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>0.004363636363636364</v>
       </c>
       <c r="H20" t="n">
         <v>0.9</v>
@@ -1022,14 +1022,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>24.283:77.907</t>
+          <t>24.273:77.941</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G21" t="n">
-        <v>0.001714285714285714</v>
+        <v>0.0032</v>
       </c>
       <c r="H21" t="n">
         <v>0.9</v>
@@ -1050,14 +1050,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>25.021:77.968</t>
+          <t>25.112:77.812</t>
         </is>
       </c>
       <c r="F22" t="n">
         <v>0.001</v>
       </c>
       <c r="G22" t="n">
-        <v>0.001714285714285714</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H22" t="n">
         <v>0.9</v>
@@ -1078,14 +1078,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>28.008:89.388</t>
+          <t>27.034:89.447</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.001</v>
+        <v>0.004</v>
       </c>
       <c r="G23" t="n">
-        <v>0.001714285714285714</v>
+        <v>0.004363636363636364</v>
       </c>
       <c r="H23" t="n">
         <v>0.9</v>
@@ -1106,14 +1106,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>29.862:95.615</t>
+          <t>30.063:95.267</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="G24" t="n">
-        <v>0.002666666666666667</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H24" t="n">
         <v>0.9</v>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>28.328:94.799</t>
+          <t>28.317:94.733</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1218,14 +1218,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>48.839:64.938</t>
+          <t>48.818:65.167</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H2" t="n">
         <v>0.9</v>
@@ -1246,7 +1246,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>54.839:87.521</t>
+          <t>54.899:87.382</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -1274,14 +1274,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>57.327:99.927</t>
+          <t>57.51:99.398</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.0016</v>
       </c>
       <c r="H4" t="n">
         <v>0.9</v>
@@ -1302,14 +1302,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>59.891:110.891</t>
+          <t>59.849:111.017</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.001333333333333333</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
         <v>0.9</v>
@@ -1330,14 +1330,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>61.93:118.385</t>
+          <t>61.935:118.336</t>
         </is>
       </c>
       <c r="F6" t="n">
         <v>0.001</v>
       </c>
       <c r="G6" t="n">
-        <v>0.001333333333333333</v>
+        <v>0.0016</v>
       </c>
       <c r="H6" t="n">
         <v>0.9</v>
@@ -1358,14 +1358,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>63.875:129.443</t>
+          <t>64.008:129.134</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G7" t="n">
-        <v>0.001333333333333333</v>
+        <v>0.002</v>
       </c>
       <c r="H7" t="n">
         <v>0.9</v>
@@ -1386,14 +1386,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>66.589:136.918</t>
+          <t>65.889:136.761</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0.9</v>
@@ -1414,14 +1414,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>66.86:142.047</t>
+          <t>66.92:142.203</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.001333333333333333</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
         <v>0.9</v>
@@ -1442,14 +1442,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>69.007:147.534</t>
+          <t>68.751:147.434</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H10" t="n">
         <v>0.9</v>
@@ -1470,14 +1470,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>69.912:154.254</t>
+          <t>69.517:154.609</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00208695652173913</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>0.9</v>
@@ -1498,14 +1498,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>71.119:158.024</t>
+          <t>72.373:157.663</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="G12" t="n">
-        <v>0.00208695652173913</v>
+        <v>0.0016</v>
       </c>
       <c r="H12" t="n">
         <v>0.9</v>
@@ -1526,14 +1526,14 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>72.859:167.093</t>
+          <t>73.83:167.036</t>
         </is>
       </c>
       <c r="F13" t="n">
         <v>0.001</v>
       </c>
       <c r="G13" t="n">
-        <v>0.001333333333333333</v>
+        <v>0.0016</v>
       </c>
       <c r="H13" t="n">
         <v>0.9</v>
@@ -1554,14 +1554,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>72.807:167.625</t>
+          <t>72.648:167.499</t>
         </is>
       </c>
       <c r="F14" t="n">
         <v>0.002</v>
       </c>
       <c r="G14" t="n">
-        <v>0.00208695652173913</v>
+        <v>0.002</v>
       </c>
       <c r="H14" t="n">
         <v>0.9</v>
@@ -1582,14 +1582,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>75.855:183.615</t>
+          <t>75.534:185.303</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.001333333333333333</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
         <v>0.9</v>
@@ -1610,14 +1610,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>76.503:176.342</t>
+          <t>76.663:176.855</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="G16" t="n">
-        <v>0.00208695652173913</v>
+        <v>0.0016</v>
       </c>
       <c r="H16" t="n">
         <v>0.9</v>
@@ -1638,14 +1638,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>76.53:182.473</t>
+          <t>76.307:182.908</t>
         </is>
       </c>
       <c r="F17" t="n">
         <v>0.001</v>
       </c>
       <c r="G17" t="n">
-        <v>0.001333333333333333</v>
+        <v>0.0016</v>
       </c>
       <c r="H17" t="n">
         <v>0.9</v>
@@ -1666,7 +1666,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>79.853:195.983</t>
+          <t>80.109:195.546</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1694,14 +1694,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>79.466:197.761</t>
+          <t>80.766:198.755</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G19" t="n">
-        <v>0.001333333333333333</v>
+        <v>0.002</v>
       </c>
       <c r="H19" t="n">
         <v>0.9</v>
@@ -1722,14 +1722,14 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>80.449:201.234</t>
+          <t>79.448:201.431</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H20" t="n">
         <v>0.9</v>
@@ -1750,14 +1750,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>83.115:207.349</t>
+          <t>83.258:207.302</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G21" t="n">
-        <v>0.001333333333333333</v>
+        <v>0.002</v>
       </c>
       <c r="H21" t="n">
         <v>0.9</v>
@@ -1778,14 +1778,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>84.314:211.553</t>
+          <t>84.105:211.546</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>0.00208695652173913</v>
+        <v>0</v>
       </c>
       <c r="H22" t="n">
         <v>0.9</v>
@@ -1806,14 +1806,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>84.602:221.113</t>
+          <t>84.597:221.404</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G23" t="n">
-        <v>0.001333333333333333</v>
+        <v>0.002</v>
       </c>
       <c r="H23" t="n">
         <v>0.9</v>
@@ -1834,14 +1834,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>86.561:231.532</t>
+          <t>86.254:230.906</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G24" t="n">
-        <v>0.001333333333333333</v>
+        <v>0.002</v>
       </c>
       <c r="H24" t="n">
         <v>0.9</v>
@@ -1862,14 +1862,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>89.903:239.863</t>
+          <t>90.546:240.257</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>0.0016</v>
       </c>
       <c r="H25" t="n">
         <v>0.9</v>
@@ -1946,7 +1946,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>142.98:573.714</t>
+          <t>139.505:574.118</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -1974,14 +1974,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>132.084:577.725</t>
+          <t>137.29:573.658</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.001411764705882353</v>
       </c>
       <c r="H3" t="n">
         <v>0.9</v>
@@ -2002,14 +2002,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>142.317:575.576</t>
+          <t>142.719:574.898</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="G4" t="n">
-        <v>0.002285714285714286</v>
+        <v>0.001411764705882353</v>
       </c>
       <c r="H4" t="n">
         <v>0.9</v>
@@ -2030,14 +2030,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>142.623:585.239</t>
+          <t>143.294:591.605</t>
         </is>
       </c>
       <c r="F5" t="n">
         <v>0.001</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0016</v>
+        <v>0.001411764705882353</v>
       </c>
       <c r="H5" t="n">
         <v>0.9</v>
@@ -2058,14 +2058,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>143.872:593.456</t>
+          <t>142.879:593.515</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="G6" t="n">
-        <v>0.002285714285714286</v>
+        <v>0.001411764705882353</v>
       </c>
       <c r="H6" t="n">
         <v>0.9</v>
@@ -2086,14 +2086,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>144.441:589.541</t>
+          <t>144.508:589.576</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0016</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>0.9</v>
@@ -2114,14 +2114,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>151.267:623.11</t>
+          <t>149.96:623.069</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H8" t="n">
         <v>0.9</v>
@@ -2142,14 +2142,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>152.404:620.613</t>
+          <t>152.032:621.023</t>
         </is>
       </c>
       <c r="F9" t="n">
         <v>0.002</v>
       </c>
       <c r="G9" t="n">
-        <v>0.002285714285714286</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H9" t="n">
         <v>0.9</v>
@@ -2170,7 +2170,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>147.506:610.227</t>
+          <t>150.067:609.831</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -2198,14 +2198,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>149.276:627.385</t>
+          <t>153.689:627.757</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0016</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H11" t="n">
         <v>0.9</v>
@@ -2226,14 +2226,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>150.161:612.445</t>
+          <t>151.025:612.016</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.001411764705882353</v>
       </c>
       <c r="H12" t="n">
         <v>0.9</v>
@@ -2254,14 +2254,14 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>144.834:599.881</t>
+          <t>142.366:599.705</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="G13" t="n">
-        <v>0.003</v>
+        <v>0.001411764705882353</v>
       </c>
       <c r="H13" t="n">
         <v>0.9</v>
@@ -2282,14 +2282,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>137.033:598.961</t>
+          <t>142.033:599.206</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0016</v>
+        <v>0.003</v>
       </c>
       <c r="H14" t="n">
         <v>0.9</v>
@@ -2310,14 +2310,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>151.664:612.125</t>
+          <t>150.899:613.81</t>
         </is>
       </c>
       <c r="F15" t="n">
         <v>0.002</v>
       </c>
       <c r="G15" t="n">
-        <v>0.002285714285714286</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H15" t="n">
         <v>0.9</v>
@@ -2338,14 +2338,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>149.671:621.72</t>
+          <t>150.581:622.104</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>0.001411764705882353</v>
       </c>
       <c r="H16" t="n">
         <v>0.9</v>
@@ -2366,14 +2366,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>149.673:623.991</t>
+          <t>156.254:623.61</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0016</v>
+        <v>0.003</v>
       </c>
       <c r="H17" t="n">
         <v>0.9</v>
@@ -2394,14 +2394,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>148.959:625.609</t>
+          <t>150.427:626.825</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="G18" t="n">
-        <v>0.003</v>
+        <v>0.001411764705882353</v>
       </c>
       <c r="H18" t="n">
         <v>0.9</v>
@@ -2422,14 +2422,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>147.507:622.889</t>
+          <t>155.794:622.836</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0.002285714285714286</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
         <v>0.9</v>
@@ -2450,7 +2450,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>150.152:622.039</t>
+          <t>152.943:621.634</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -2478,14 +2478,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>154.327:628.131</t>
+          <t>154.388:626.711</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H21" t="n">
         <v>0.9</v>
@@ -2506,14 +2506,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>154.647:638.111</t>
+          <t>154.674:640.594</t>
         </is>
       </c>
       <c r="F22" t="n">
         <v>0.001</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0016</v>
+        <v>0.001411764705882353</v>
       </c>
       <c r="H22" t="n">
         <v>0.9</v>
@@ -2534,14 +2534,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>150.989:611.549</t>
+          <t>150.524:613.823</t>
         </is>
       </c>
       <c r="F23" t="n">
         <v>0.001</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0016</v>
+        <v>0.001411764705882353</v>
       </c>
       <c r="H23" t="n">
         <v>0.9</v>
@@ -2562,14 +2562,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>144.544:581.39</t>
+          <t>147.921:581.39</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.002285714285714286</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
         <v>0.9</v>
@@ -2590,14 +2590,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>142.344:582.931</t>
+          <t>139.811:580.348</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="G25" t="n">
-        <v>0.003</v>
+        <v>0.001411764705882353</v>
       </c>
       <c r="H25" t="n">
         <v>0.9</v>
@@ -2674,14 +2674,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>29.0:39.351</t>
+          <t>28.897:39.44</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.01</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01043478260869565</v>
+        <v>0.009391304347826085</v>
       </c>
       <c r="H2" t="n">
         <v>0.9</v>
@@ -2702,14 +2702,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>27.468:39.466</t>
+          <t>27.581:39.531</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.033</v>
+        <v>0.029</v>
       </c>
       <c r="G3" t="n">
-        <v>0.033</v>
+        <v>0.029</v>
       </c>
       <c r="H3" t="n">
         <v>0.9</v>
@@ -2730,14 +2730,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>29.382:44.77</t>
+          <t>29.388:44.824</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.002</v>
+        <v>0.006</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0024</v>
+        <v>0.006545454545454546</v>
       </c>
       <c r="H4" t="n">
         <v>0.9</v>
@@ -2758,14 +2758,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>33.428:57.796</t>
+          <t>33.209:58.302</t>
         </is>
       </c>
       <c r="F5" t="n">
         <v>0.002</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0024</v>
+        <v>0.002666666666666667</v>
       </c>
       <c r="H5" t="n">
         <v>0.9</v>
@@ -2786,14 +2786,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>37.256:71.012</t>
+          <t>36.665:71.029</t>
         </is>
       </c>
       <c r="F6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G6" t="n">
         <v>0.002</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.0024</v>
       </c>
       <c r="H6" t="n">
         <v>0.9</v>
@@ -2814,14 +2814,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>40.302:88.635</t>
+          <t>39.786:88.566</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.0036</v>
       </c>
       <c r="H7" t="n">
         <v>0.9</v>
@@ -2842,14 +2842,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>43.029:99.234</t>
+          <t>42.843:99.215</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.001846153846153846</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0.9</v>
@@ -2870,14 +2870,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>46.403:119.07</t>
+          <t>46.6:118.993</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0024</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
         <v>0.9</v>
@@ -2898,14 +2898,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>49.908:130.917</t>
+          <t>50.404:131.183</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.001846153846153846</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
         <v>0.9</v>
@@ -2926,14 +2926,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>54.316:148.08</t>
+          <t>53.464:147.835</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.001846153846153846</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>0.9</v>
@@ -2954,14 +2954,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>58.014:164.481</t>
+          <t>59.139:165.34</t>
         </is>
       </c>
       <c r="F12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G12" t="n">
         <v>0.002</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.0024</v>
       </c>
       <c r="H12" t="n">
         <v>0.9</v>
@@ -2982,14 +2982,14 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>64.238:190.007</t>
+          <t>63.799:188.964</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G13" t="n">
-        <v>0.001846153846153846</v>
+        <v>0.002666666666666667</v>
       </c>
       <c r="H13" t="n">
         <v>0.9</v>
@@ -3010,14 +3010,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>69.086:204.891</t>
+          <t>68.483:203.989</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.001846153846153846</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
         <v>0.9</v>
@@ -3038,14 +3038,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>74.486:234.658</t>
+          <t>73.279:234.27</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>0.002666666666666667</v>
       </c>
       <c r="H15" t="n">
         <v>0.9</v>
@@ -3066,14 +3066,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>81.577:263.082</t>
+          <t>82.043:261.165</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.004</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.004363636363636364</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
         <v>0.9</v>
@@ -3094,14 +3094,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>84.134:290.469</t>
+          <t>85.226:290.648</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H17" t="n">
         <v>0.9</v>
@@ -3122,14 +3122,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>99.133:353.764</t>
+          <t>100.5:356.385</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="G18" t="n">
-        <v>0.003428571428571429</v>
+        <v>0.002666666666666667</v>
       </c>
       <c r="H18" t="n">
         <v>0.9</v>
@@ -3150,14 +3150,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>117.827:434.355</t>
+          <t>117.65:442.193</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>0.004571428571428572</v>
       </c>
       <c r="H19" t="n">
         <v>0.9</v>
@@ -3178,14 +3178,14 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>123.97:437.538</t>
+          <t>124.561:435.801</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G20" t="n">
-        <v>0.001846153846153846</v>
+        <v>0.002666666666666667</v>
       </c>
       <c r="H20" t="n">
         <v>0.9</v>
@@ -3206,14 +3206,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>137.394:513.176</t>
+          <t>134.07:512.995</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0024</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
         <v>0.9</v>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>144.996:533.581</t>
+          <t>146.606:534.372</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -3262,14 +3262,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>173.803:638.343</t>
+          <t>164.085:637.571</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>0.002666666666666667</v>
       </c>
       <c r="H23" t="n">
         <v>0.9</v>
@@ -3290,14 +3290,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>189.966:694.527</t>
+          <t>187.577:694.7</t>
         </is>
       </c>
       <c r="F24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G24" t="n">
         <v>0.002</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.0024</v>
       </c>
       <c r="H24" t="n">
         <v>0.9</v>
@@ -3318,14 +3318,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>177.458:700.192</t>
+          <t>179.171:699.098</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="G25" t="n">
-        <v>0.001846153846153846</v>
+        <v>0.0036</v>
       </c>
       <c r="H25" t="n">
         <v>0.9</v>
@@ -3402,14 +3402,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>88.703:150.469</t>
+          <t>88.151:150.163</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G2" t="n">
-        <v>0.001263157894736842</v>
+        <v>0.002285714285714286</v>
       </c>
       <c r="H2" t="n">
         <v>0.9</v>
@@ -3430,14 +3430,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>122.585:284.918</t>
+          <t>121.736:284.275</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="G3" t="n">
-        <v>0.001263157894736842</v>
+        <v>0.003130434782608696</v>
       </c>
       <c r="H3" t="n">
         <v>0.9</v>
@@ -3458,14 +3458,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>142.477:379.171</t>
+          <t>143.021:378.154</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G4" t="n">
-        <v>0.001263157894736842</v>
+        <v>0.002285714285714286</v>
       </c>
       <c r="H4" t="n">
         <v>0.9</v>
@@ -3486,14 +3486,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>157.207:454.279</t>
+          <t>162.365:454.934</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="G5" t="n">
-        <v>0.003130434782608696</v>
+        <v>0.001714285714285714</v>
       </c>
       <c r="H5" t="n">
         <v>0.9</v>
@@ -3514,14 +3514,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>174.128:519.452</t>
+          <t>177.503:521.809</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.002181818181818182</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>0.9</v>
@@ -3542,14 +3542,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>190.029:598.604</t>
+          <t>191.241:594.17</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.001263157894736842</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>0.9</v>
@@ -3570,14 +3570,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>204.954:646.376</t>
+          <t>210.487:646.639</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.002181818181818182</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0.9</v>
@@ -3598,14 +3598,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>214.7:682.93</t>
+          <t>215.843:686.278</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>0.001714285714285714</v>
       </c>
       <c r="H9" t="n">
         <v>0.9</v>
@@ -3626,14 +3626,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>229.971:729.055</t>
+          <t>223.179:728.818</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G10" t="n">
-        <v>0.001263157894736842</v>
+        <v>0.002285714285714286</v>
       </c>
       <c r="H10" t="n">
         <v>0.9</v>
@@ -3654,14 +3654,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>233.573:777.254</t>
+          <t>232.72:777.673</t>
         </is>
       </c>
       <c r="F11" t="n">
         <v>0.002</v>
       </c>
       <c r="G11" t="n">
-        <v>0.002181818181818182</v>
+        <v>0.002285714285714286</v>
       </c>
       <c r="H11" t="n">
         <v>0.9</v>
@@ -3682,14 +3682,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>242.462:781.762</t>
+          <t>239.893:780.984</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.001714285714285714</v>
       </c>
       <c r="H12" t="n">
         <v>0.9</v>
@@ -3710,14 +3710,14 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>248.248:847.481</t>
+          <t>248.024:845.539</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>0.001714285714285714</v>
       </c>
       <c r="H13" t="n">
         <v>0.9</v>
@@ -3738,14 +3738,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>265.153:881.714</t>
+          <t>265.027:882.309</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="G14" t="n">
-        <v>0.001263157894736842</v>
+        <v>0.003130434782608696</v>
       </c>
       <c r="H14" t="n">
         <v>0.9</v>
@@ -3766,14 +3766,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>250.401:882.22</t>
+          <t>258.589:882.218</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>0.001714285714285714</v>
       </c>
       <c r="H15" t="n">
         <v>0.9</v>
@@ -3794,14 +3794,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>253.895:834.758</t>
+          <t>253.666:835.136</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="H16" t="n">
         <v>0.9</v>
@@ -3822,14 +3822,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>258.616:879.51</t>
+          <t>260.485:876.224</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G17" t="n">
-        <v>0.001263157894736842</v>
+        <v>0.002285714285714286</v>
       </c>
       <c r="H17" t="n">
         <v>0.9</v>
@@ -3850,14 +3850,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>268.733:925.261</t>
+          <t>269.95:926.175</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>0.002285714285714286</v>
       </c>
       <c r="H18" t="n">
         <v>0.9</v>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>272.188:927.52</t>
+          <t>274.326:928.837</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -3906,14 +3906,14 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>271.737:951.136</t>
+          <t>265.622:952.452</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0.001263157894736842</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
         <v>0.9</v>
@@ -3934,14 +3934,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>286.867:974.99</t>
+          <t>285.954:977.19</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="G21" t="n">
-        <v>0.001263157894736842</v>
+        <v>0.002285714285714286</v>
       </c>
       <c r="H21" t="n">
         <v>0.9</v>
@@ -3962,14 +3962,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>281.739:972.125</t>
+          <t>287.361:971.405</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>0.001714285714285714</v>
       </c>
       <c r="H22" t="n">
         <v>0.9</v>
@@ -3990,14 +3990,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>287.023:1015.663</t>
+          <t>284.403:1015.853</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="G23" t="n">
-        <v>0.004</v>
+        <v>0.001714285714285714</v>
       </c>
       <c r="H23" t="n">
         <v>0.9</v>
@@ -4018,14 +4018,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>290.707:1036.089</t>
+          <t>295.761:1038.387</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.001263157894736842</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
         <v>0.9</v>
@@ -4046,14 +4046,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>302.155:1068.221</t>
+          <t>304.819:1068.281</t>
         </is>
       </c>
       <c r="F25" t="n">
         <v>0.001</v>
       </c>
       <c r="G25" t="n">
-        <v>0.001263157894736842</v>
+        <v>0.001714285714285714</v>
       </c>
       <c r="H25" t="n">
         <v>0.9</v>
@@ -4130,14 +4130,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>438.176:1847.889</t>
+          <t>449.728:1853.877</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H2" t="n">
         <v>0.9</v>
@@ -4158,14 +4158,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>482.047:2037.912</t>
+          <t>488.355:2001.912</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="G3" t="n">
-        <v>0.002285714285714286</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H3" t="n">
         <v>0.9</v>
@@ -4186,14 +4186,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>517.243:2091.952</t>
+          <t>518.283:2092.158</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0015</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>0.9</v>
@@ -4214,14 +4214,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>499.013:2093.451</t>
+          <t>507.75:2092.615</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H5" t="n">
         <v>0.9</v>
@@ -4242,14 +4242,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>511.186:2105.635</t>
+          <t>507.913:2105.487</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H6" t="n">
         <v>0.9</v>
@@ -4270,7 +4270,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>519.821:2128.775</t>
+          <t>507.998:2127.453</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -4298,7 +4298,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>445.058:1776.095</t>
+          <t>443.808:1773.553</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -4326,14 +4326,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>441.906:1773.397</t>
+          <t>430.805:1775.426</t>
         </is>
       </c>
       <c r="F9" t="n">
         <v>0.001</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0015</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H9" t="n">
         <v>0.9</v>
@@ -4354,7 +4354,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>430.581:1789.63</t>
+          <t>432.187:1787.617</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -4382,14 +4382,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>431.509:1783.075</t>
+          <t>436.614:1782.169</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="G11" t="n">
-        <v>0.002285714285714286</v>
+        <v>0.003</v>
       </c>
       <c r="H11" t="n">
         <v>0.9</v>
@@ -4410,14 +4410,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>438.535:1746.508</t>
+          <t>442.801:1753.211</t>
         </is>
       </c>
       <c r="F12" t="n">
         <v>0.001</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0015</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H12" t="n">
         <v>0.9</v>
@@ -4438,14 +4438,14 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>403.755:1718.3</t>
+          <t>408.979:1719.305</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0015</v>
+        <v>0.003</v>
       </c>
       <c r="H13" t="n">
         <v>0.9</v>
@@ -4466,14 +4466,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>399.563:1643.652</t>
+          <t>412.107:1645.162</t>
         </is>
       </c>
       <c r="F14" t="n">
         <v>0.001</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0015</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H14" t="n">
         <v>0.9</v>
@@ -4494,14 +4494,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>429.804:1699.342</t>
+          <t>416.677:1694.725</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="G15" t="n">
-        <v>0.003130434782608696</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H15" t="n">
         <v>0.9</v>
@@ -4522,14 +4522,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>423.062:1733.453</t>
+          <t>428.225:1734.683</t>
         </is>
       </c>
       <c r="F16" t="n">
         <v>0.002</v>
       </c>
       <c r="G16" t="n">
-        <v>0.002285714285714286</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H16" t="n">
         <v>0.9</v>
@@ -4550,14 +4550,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>427.275:1738.867</t>
+          <t>433.7:1738.285</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="G17" t="n">
-        <v>0.003130434782608696</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H17" t="n">
         <v>0.9</v>
@@ -4578,14 +4578,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>425.15:1705.114</t>
+          <t>423.428:1704.384</t>
         </is>
       </c>
       <c r="F18" t="n">
         <v>0.001</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0015</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H18" t="n">
         <v>0.9</v>
@@ -4606,14 +4606,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>413.96:1670.418</t>
+          <t>411.086:1673.588</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0.002285714285714286</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
         <v>0.9</v>
@@ -4634,14 +4634,14 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>422.157:1700.997</t>
+          <t>426.222:1706.283</t>
         </is>
       </c>
       <c r="F20" t="n">
         <v>0.001</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0015</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H20" t="n">
         <v>0.9</v>
@@ -4662,14 +4662,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>418.28:1667.388</t>
+          <t>403.897:1669.233</t>
         </is>
       </c>
       <c r="F21" t="n">
         <v>0.001</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0015</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H21" t="n">
         <v>0.9</v>
@@ -4690,14 +4690,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>412.093:1730.758</t>
+          <t>410.565:1727.319</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="G22" t="n">
-        <v>0.002285714285714286</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H22" t="n">
         <v>0.9</v>
@@ -4718,14 +4718,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>411.2:1639.741</t>
+          <t>409.371:1635.843</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>0.002181818181818182</v>
       </c>
       <c r="H23" t="n">
         <v>0.9</v>
@@ -4746,14 +4746,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>397.228:1559.853</t>
+          <t>394.383:1560.768</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="G24" t="n">
-        <v>0.004</v>
+        <v>0.001263157894736842</v>
       </c>
       <c r="H24" t="n">
         <v>0.9</v>
@@ -4774,14 +4774,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>381.891:1564.053</t>
+          <t>381.245:1563.413</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0015</v>
+        <v>0</v>
       </c>
       <c r="H25" t="n">
         <v>0.9</v>

</xml_diff>